<commit_message>
Changes to support MBuck's  updated CEDD  ontology. Primarily, value sets and demographic codes of type IVL_TS
Former-commit-id: 64f6205312f43620e5c5e8ebb170d40d28173d72
</commit_message>
<xml_diff>
--- a/source/Translators/I2B2 HQMF Transforms/supported_mappings.xlsx
+++ b/source/Translators/I2B2 HQMF Transforms/supported_mappings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22624"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="26480" windowHeight="15300"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="26480" windowHeight="15300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="82">
   <si>
     <t>\categoryAttribute\socialHistory\socialHistoryType_code\ (and _text)</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Encounter (code/value - not age at visit or length of stay)</t>
   </si>
   <si>
-    <t>NEW! (with limitation in CEDD)</t>
-  </si>
-  <si>
     <t>Date and time modifiers</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
     <t>Results</t>
   </si>
   <si>
-    <t>ALMOST BIDIRECTIONAL - BUG IN APPLIED PATH DUE TO REUSING CRITERIA</t>
-  </si>
-  <si>
     <t>Social History</t>
   </si>
   <si>
@@ -184,9 +178,6 @@
     <t>Diagnosis - type code</t>
   </si>
   <si>
-    <t>NEW! - but might be incorrect</t>
-  </si>
-  <si>
     <t>*_code (with basecode starting with CEDD:)</t>
   </si>
   <si>
@@ -250,9 +241,6 @@
     <t>Length of stay</t>
   </si>
   <si>
-    <t xml:space="preserve">NOTE: temporal constraints in items handled separately. </t>
-  </si>
-  <si>
     <t>\CEDD\patientInformation\visitAge_value\</t>
   </si>
   <si>
@@ -263,6 +251,21 @@
   </si>
   <si>
     <t>NOT IMPLEMENTED, not priority</t>
+  </si>
+  <si>
+    <t>*_code (with basecode start with OID:)</t>
+  </si>
+  <si>
+    <t>Value sets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE: temporal constraints in items work. </t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>NEW! - but might be incorrect HQMF</t>
   </si>
 </sst>
 </file>
@@ -275,7 +278,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -295,6 +298,20 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -352,7 +369,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -371,8 +388,14 @@
     <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -418,12 +441,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
     <cellStyle name="Comma" xfId="4"/>
     <cellStyle name="Comma[0]" xfId="5"/>
     <cellStyle name="Currency" xfId="2"/>
     <cellStyle name="Currency[0]" xfId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1"/>
   </cellStyles>
@@ -783,7 +814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -793,7 +824,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="12">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="12">
@@ -803,17 +834,17 @@
     </row>
     <row r="4" spans="1:1" ht="24">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="24">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="24">
       <c r="A6" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -829,11 +860,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P107"/>
+  <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -842,24 +873,25 @@
     <col min="2" max="2" width="57" customWidth="1"/>
     <col min="3" max="3" width="25.1640625" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="16" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="16" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="24">
@@ -867,385 +899,395 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="24">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="36">
-      <c r="A4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="48">
-      <c r="A5" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="12">
+      <c r="A4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="36">
+      <c r="A5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="48">
+      <c r="A6" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="12">
-      <c r="A6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="12">
       <c r="A7" s="4" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="12">
+      <c r="A8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="24">
-      <c r="A8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:6" ht="24">
+      <c r="A9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E9" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="12">
+      <c r="A10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="24">
+      <c r="A11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="12">
+      <c r="A12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="24">
+      <c r="A13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="24">
+      <c r="A14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="24">
+      <c r="A15" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="12">
-      <c r="A9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="24">
-      <c r="A10" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="12">
-      <c r="A11" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="24">
-      <c r="A12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="36">
-      <c r="A13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="24">
-      <c r="A14" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="12">
-      <c r="A15" s="9" t="s">
+      <c r="E15" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="12">
+      <c r="A16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="48">
-      <c r="A16" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="36">
-      <c r="A17" s="4" t="s">
-        <v>50</v>
+    <row r="17" spans="1:5" ht="48">
+      <c r="A17" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="24">
+      <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="36">
-      <c r="A18" s="4" t="s">
-        <v>75</v>
+      <c r="B18" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="12">
-      <c r="A19" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="24">
-      <c r="A20" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="24">
+      <c r="A19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="12">
+      <c r="A20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="24">
+      <c r="A21" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="12">
-      <c r="A22" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>34</v>
+      <c r="E21" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="12">
-      <c r="A23" s="4"/>
+      <c r="A23" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B23" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="24">
-      <c r="A24" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="12">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="24">
+      <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="24">
-      <c r="A25" s="4"/>
       <c r="B25" s="6" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="24">
       <c r="A26" s="4"/>
       <c r="B26" s="6" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="24">
       <c r="A27" s="4"/>
       <c r="B27" s="6" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="24">
       <c r="A28" s="4"/>
       <c r="B28" s="6" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="12">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="24">
       <c r="A29" s="4"/>
       <c r="B29" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="24">
+        <v>42</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="12">
       <c r="A30" s="4"/>
       <c r="B30" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="12">
+        <v>36</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="24">
       <c r="A31" s="4"/>
       <c r="B31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="12">
+      <c r="A32" s="4"/>
+      <c r="B32" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="12">
+      <c r="A33" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="12">
+      <c r="A34" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="12">
-      <c r="A32" s="9" t="s">
+      <c r="B34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" ht="60">
-      <c r="A33" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" ht="12">
-      <c r="A35" s="4"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
     </row>
     <row r="36" spans="1:16" ht="12">
       <c r="A36" s="4"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
     </row>
     <row r="37" spans="1:16" ht="12">
       <c r="A37" s="4"/>
@@ -1262,8 +1304,8 @@
     <row r="41" spans="1:16" ht="12">
       <c r="A41" s="4"/>
     </row>
-    <row r="43" spans="1:16" ht="12">
-      <c r="A43" s="4"/>
+    <row r="42" spans="1:16" ht="12">
+      <c r="A42" s="4"/>
     </row>
     <row r="44" spans="1:16" ht="12">
       <c r="A44" s="4"/>
@@ -1456,6 +1498,9 @@
     </row>
     <row r="107" spans="1:1" ht="12">
       <c r="A107" s="4"/>
+    </row>
+    <row r="108" spans="1:1" ht="12">
+      <c r="A108" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>